<commit_message>
created grasp_decoding.m and updated other scripts
updated code
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C54FBEE-9B72-401A-AE5D-5458A682ADE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E77597-4ABE-479F-928C-F8DB9AB932A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4470" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14940" yWindow="2790" windowWidth="12150" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>wrong = 9, 10</t>
+  </si>
+  <si>
+    <t>7,14</t>
+  </si>
+  <si>
+    <t>7,10</t>
+  </si>
+  <si>
+    <t>really good run</t>
   </si>
 </sst>
 </file>
@@ -408,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,6 +604,72 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20230817</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20230824</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
thresholded 20230831 session; added shadedErrorBar to path
still unable to get matlab to recognize shadedErrorBar as a function. I thought maybe updating the GitHub would help
</commit_message>
<xml_diff>
--- a/ExcelFiles/s2_good_trials_GraspObject.xlsx
+++ b/ExcelFiles/s2_good_trials_GraspObject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E77597-4ABE-479F-928C-F8DB9AB932A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FDBB81-8647-4803-B5B3-87E720EFFB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14940" yWindow="2790" windowWidth="12150" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4470" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>really good run</t>
+  </si>
+  <si>
+    <t>8,14,15,17,20</t>
+  </si>
+  <si>
+    <t>10,17,18</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,8,13</t>
+  </si>
+  <si>
+    <t>17,18</t>
   </si>
 </sst>
 </file>
@@ -108,6 +120,7 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -417,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +618,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>20230817</v>
       </c>
       <c r="B11">
@@ -668,6 +681,46 @@
       </c>
       <c r="G14" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20230831</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>